<commit_message>
Updated cases for new parameters
</commit_message>
<xml_diff>
--- a/andes/cases/ieee14/ieee14_solar.xlsx
+++ b/andes/cases/ieee14/ieee14_solar.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11108"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cuiha\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hcui7/repos/andes/andes/cases/ieee14/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07BA4A8F-8662-4216-8E15-0C907CD27A42}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08576D2F-FE9C-D74A-AC82-EA519B85B4EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3330" yWindow="3810" windowWidth="36660" windowHeight="16305" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="3380" windowWidth="33600" windowHeight="16300" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Toggler" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="260">
   <si>
     <t>uid</t>
   </si>
@@ -574,12 +574,6 @@
     <t>Accel</t>
   </si>
   <si>
-    <t>Iqmax</t>
-  </si>
-  <si>
-    <t>Iqmin</t>
-  </si>
-  <si>
     <t>REGCA1_1</t>
   </si>
   <si>
@@ -818,13 +812,16 @@
   </si>
   <si>
     <t>REECA1_1</t>
+  </si>
+  <si>
+    <t>PLflag</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1211,9 +1208,9 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1236,7 +1233,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1259,7 +1256,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1296,9 +1293,9 @@
       <selection pane="bottomLeft" activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1342,7 +1339,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1383,7 +1380,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1424,7 +1421,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1465,7 +1462,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1520,9 +1517,9 @@
       <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1575,7 +1572,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1642,9 +1639,9 @@
       <selection pane="bottomLeft" activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:26">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1724,7 +1721,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="2" spans="1:26">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1804,7 +1801,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:26">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1884,7 +1881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:26">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1978,9 +1975,9 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2006,7 +2003,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -2032,7 +2029,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -2058,7 +2055,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -2091,19 +2088,19 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC49D34E-907B-4E1F-B94C-5AE270F09226}">
-  <dimension ref="A1:X2"/>
+  <dimension ref="A1:V2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
+      <selection pane="bottomLeft" activeCell="R7" sqref="R7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="16384" width="8.85546875" style="3"/>
+    <col min="1" max="16384" width="8.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2165,30 +2162,24 @@
         <v>178</v>
       </c>
       <c r="U1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3">
+        <v>1</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>179</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="W1" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="X1" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24">
-      <c r="A2" s="2">
-        <v>0</v>
-      </c>
-      <c r="B2" s="3">
-        <v>1</v>
-      </c>
-      <c r="C2" s="3">
-        <v>1</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>181</v>
       </c>
       <c r="E2" s="3">
         <v>8</v>
@@ -2239,15 +2230,9 @@
         <v>0</v>
       </c>
       <c r="U2" s="3">
-        <v>999</v>
+        <v>0</v>
       </c>
       <c r="V2" s="3">
-        <v>-999</v>
-      </c>
-      <c r="W2" s="3">
-        <v>0</v>
-      </c>
-      <c r="X2" s="3">
         <v>0.25</v>
       </c>
     </row>
@@ -2260,17 +2245,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A35E049C-6957-482F-A25F-1186A8D8FFB3}">
   <dimension ref="A1:BD2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="AG3" sqref="AG3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="16384" width="8.85546875" style="3"/>
+    <col min="1" max="16384" width="8.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:56">
+    <row r="1" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2284,70 +2269,70 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>50</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="O1" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="Q1" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="O1" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="Q1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="X1" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="Y1" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>229</v>
-      </c>
-      <c r="X1" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="Y1" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="Z1" s="2" t="s">
-        <v>231</v>
       </c>
       <c r="AA1" s="2" t="s">
         <v>123</v>
@@ -2356,102 +2341,102 @@
         <v>124</v>
       </c>
       <c r="AC1" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="AD1" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="AE1" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AF1" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="AE1" s="2" t="s">
+      <c r="AG1" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="AF1" s="2" t="s">
+      <c r="AH1" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="AG1" s="2" t="s">
+      <c r="AI1" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="AH1" s="2" t="s">
+      <c r="AJ1" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="AI1" s="2" t="s">
+      <c r="AK1" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="AJ1" s="2" t="s">
+      <c r="AL1" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="AK1" s="2" t="s">
+      <c r="AM1" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="AL1" s="2" t="s">
+      <c r="AN1" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="AM1" s="2" t="s">
+      <c r="AO1" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="AN1" s="2" t="s">
+      <c r="AP1" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="AO1" s="2" t="s">
+      <c r="AQ1" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="AP1" s="2" t="s">
+      <c r="AR1" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="AQ1" s="2" t="s">
+      <c r="AS1" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="AR1" s="2" t="s">
+      <c r="AT1" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="AS1" s="2" t="s">
+      <c r="AU1" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="AT1" s="2" t="s">
+      <c r="AV1" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="AU1" s="2" t="s">
+      <c r="AW1" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="AV1" s="2" t="s">
+      <c r="AX1" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="AW1" s="2" t="s">
+      <c r="AY1" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="AX1" s="2" t="s">
+      <c r="AZ1" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="AY1" s="2" t="s">
+      <c r="BA1" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="AZ1" s="2" t="s">
+      <c r="BB1" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="BA1" s="2" t="s">
+      <c r="BC1" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="BB1" s="2" t="s">
+      <c r="BD1" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="BC1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:56" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3">
+        <v>1</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>258</v>
-      </c>
-      <c r="BD1" s="2" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="2" spans="1:56">
-      <c r="A2" s="2">
-        <v>0</v>
-      </c>
-      <c r="B2" s="3">
-        <v>1</v>
-      </c>
-      <c r="C2" s="3">
-        <v>1</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>260</v>
       </c>
       <c r="E2" s="3">
         <v>1</v>
@@ -2614,19 +2599,19 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCA4D5BF-F19A-4972-8DAC-8235C5F51DC0}">
-  <dimension ref="A1:AL2"/>
+  <dimension ref="A1:AM2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
+      <selection pane="bottomLeft" activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="16384" width="8.85546875" style="3"/>
+    <col min="1" max="16384" width="8.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38">
+    <row r="1" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2640,120 +2625,123 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>50</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="L1" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="N1" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="L1" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="M1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="AB1" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AC1" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AD1" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AE1" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AF1" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AG1" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="AE1" s="2" t="s">
+      <c r="AH1" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="AF1" s="2" t="s">
+      <c r="AI1" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="AG1" s="2" t="s">
+      <c r="AJ1" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="AH1" s="2" t="s">
+      <c r="AK1" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="AL1" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="AI1" s="2" t="s">
+      <c r="AM1" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="AJ1" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="AK1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3">
+        <v>1</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>211</v>
-      </c>
-      <c r="AL1" s="2" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="2" spans="1:38">
-      <c r="A2" s="2">
-        <v>0</v>
-      </c>
-      <c r="B2" s="3">
-        <v>1</v>
-      </c>
-      <c r="C2" s="3">
-        <v>1</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>213</v>
       </c>
       <c r="E2" s="3">
         <v>1</v>
@@ -2771,78 +2759,81 @@
         <v>0</v>
       </c>
       <c r="L2" s="3">
+        <v>0</v>
+      </c>
+      <c r="M2" s="3">
         <v>0.02</v>
       </c>
-      <c r="M2" s="3">
-        <v>1</v>
-      </c>
       <c r="N2" s="3">
+        <v>1</v>
+      </c>
+      <c r="O2" s="3">
         <v>0.1</v>
       </c>
-      <c r="O2" s="3">
-        <v>1</v>
-      </c>
       <c r="P2" s="3">
         <v>1</v>
       </c>
       <c r="Q2" s="3">
+        <v>1</v>
+      </c>
+      <c r="R2" s="3">
         <v>0.8</v>
       </c>
-      <c r="T2" s="3">
-        <v>1</v>
-      </c>
       <c r="U2" s="3">
+        <v>1</v>
+      </c>
+      <c r="V2" s="3">
         <v>999</v>
       </c>
-      <c r="V2" s="3">
+      <c r="W2" s="3">
         <v>-999</v>
       </c>
-      <c r="W2" s="3">
+      <c r="X2" s="3">
         <v>-0.02</v>
       </c>
-      <c r="X2" s="3">
+      <c r="Y2" s="3">
         <v>0.02</v>
       </c>
-      <c r="Y2" s="3">
+      <c r="Z2" s="3">
         <v>999</v>
       </c>
-      <c r="Z2" s="3">
+      <c r="AA2" s="3">
         <v>-999</v>
       </c>
-      <c r="AA2" s="3">
-        <v>1</v>
-      </c>
       <c r="AB2" s="3">
+        <v>1</v>
+      </c>
+      <c r="AC2" s="3">
         <v>0.1</v>
       </c>
-      <c r="AC2" s="3">
+      <c r="AD2" s="3">
         <v>0.02</v>
       </c>
-      <c r="AD2" s="3">
+      <c r="AE2" s="3">
         <v>-0.01</v>
       </c>
-      <c r="AE2" s="3">
+      <c r="AF2" s="3">
         <v>0.01</v>
       </c>
-      <c r="AF2" s="3">
+      <c r="AG2" s="3">
         <v>0.05</v>
       </c>
-      <c r="AG2" s="3">
+      <c r="AH2" s="3">
         <v>-0.05</v>
       </c>
-      <c r="AH2" s="3">
+      <c r="AI2" s="3">
         <v>999</v>
       </c>
-      <c r="AI2" s="3">
+      <c r="AJ2" s="3">
         <v>-999</v>
       </c>
-      <c r="AJ2" s="3">
+      <c r="AK2" s="3">
         <v>0.02</v>
       </c>
-      <c r="AK2" s="3">
+      <c r="AL2" s="3">
         <v>10</v>
       </c>
-      <c r="AL2" s="3">
+      <c r="AM2" s="3">
         <v>10</v>
       </c>
     </row>
@@ -2860,9 +2851,9 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2906,7 +2897,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -2950,7 +2941,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -2994,7 +2985,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -3038,7 +3029,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -3082,7 +3073,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -3126,7 +3117,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -3170,7 +3161,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -3214,7 +3205,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -3258,7 +3249,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -3302,7 +3293,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -3346,7 +3337,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -3390,7 +3381,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -3434,7 +3425,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -3478,7 +3469,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -3536,9 +3527,9 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3573,7 +3564,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -3608,7 +3599,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -3643,7 +3634,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -3678,7 +3669,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -3713,7 +3704,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -3748,7 +3739,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -3783,7 +3774,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -3818,7 +3809,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -3853,7 +3844,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -3888,7 +3879,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -3923,7 +3914,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -3972,9 +3963,9 @@
       <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4033,7 +4024,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -4089,7 +4080,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -4145,7 +4136,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -4201,7 +4192,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -4271,9 +4262,9 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4335,7 +4326,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:20">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -4408,9 +4399,9 @@
       <selection pane="bottomLeft" activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4484,7 +4475,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:24">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -4549,7 +4540,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:24">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -4614,7 +4605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:24">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -4679,7 +4670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:24">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -4744,7 +4735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:24">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -4809,7 +4800,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:24">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -4874,7 +4865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:24">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -4939,7 +4930,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:24">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -5004,7 +4995,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:24">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -5069,7 +5060,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:24">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -5134,7 +5125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:24">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -5199,7 +5190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:24">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -5264,7 +5255,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:24">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -5329,7 +5320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:24">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -5394,7 +5385,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:24">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -5459,7 +5450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:21">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -5524,7 +5515,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:21">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -5589,7 +5580,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:21">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -5654,7 +5645,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:21">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -5719,7 +5710,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:21">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -5798,9 +5789,9 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5832,7 +5823,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -5864,7 +5855,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -5910,9 +5901,9 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5926,7 +5917,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -5940,7 +5931,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -5968,9 +5959,9 @@
       <selection pane="bottomLeft" activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:28">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6056,7 +6047,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="2" spans="1:28">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -6139,7 +6130,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="3" spans="1:28">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -6222,7 +6213,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="4" spans="1:28">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -6305,7 +6296,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="5" spans="1:28">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>3</v>
       </c>

</xml_diff>